<commit_message>
Acrescentado Relatorios semanais (historico) do rendimento de cada funcionario e da equipe, num total de 4 semanas de historico.
</commit_message>
<xml_diff>
--- a/docs/SDM_Avaliacao.xlsx
+++ b/docs/SDM_Avaliacao.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Daniel Neves Camargo</t>
   </si>
@@ -73,9 +73,6 @@
   </si>
   <si>
     <t>Antonio Nery Cupolillo</t>
-  </si>
-  <si>
-    <t>Davan Martinho do Nascimento</t>
   </si>
   <si>
     <t>Yasmine Maiafaia</t>
@@ -622,10 +619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AI30"/>
+  <dimension ref="A1:AI29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -638,109 +635,109 @@
   <sheetData>
     <row r="1" spans="1:35" ht="94.5">
       <c r="A1" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AA1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AH1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="AI1" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:35">
@@ -1773,8 +1770,8 @@
       <c r="A20" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="9" t="s">
-        <v>6</v>
+      <c r="B20" s="9">
+        <v>42114</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="4"/>
@@ -1786,7 +1783,9 @@
         <v>1</v>
       </c>
       <c r="J20" s="7"/>
-      <c r="K20" s="5"/>
+      <c r="K20" s="5">
+        <v>1</v>
+      </c>
       <c r="L20" s="5"/>
       <c r="M20" s="5"/>
       <c r="N20" s="5"/>
@@ -1795,29 +1794,41 @@
       <c r="Q20" s="4"/>
       <c r="R20" s="4"/>
       <c r="S20" s="4"/>
-      <c r="T20" s="4"/>
+      <c r="T20" s="4">
+        <v>1</v>
+      </c>
       <c r="U20" s="4"/>
       <c r="V20" s="5"/>
       <c r="W20" s="5"/>
-      <c r="X20" s="5"/>
+      <c r="X20" s="5">
+        <v>1</v>
+      </c>
       <c r="Y20" s="5"/>
       <c r="Z20" s="5"/>
       <c r="AA20" s="4"/>
-      <c r="AB20" s="4"/>
+      <c r="AB20" s="4">
+        <v>1</v>
+      </c>
       <c r="AC20" s="5"/>
-      <c r="AD20" s="5"/>
+      <c r="AD20" s="5">
+        <v>1</v>
+      </c>
       <c r="AE20" s="5"/>
       <c r="AF20" s="4"/>
-      <c r="AG20" s="4"/>
+      <c r="AG20" s="4">
+        <v>1</v>
+      </c>
       <c r="AH20" s="5"/>
-      <c r="AI20" s="5"/>
+      <c r="AI20" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="21" spans="1:35">
       <c r="A21" s="10" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="9">
-        <v>42114</v>
+        <v>19287</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="4"/>
@@ -1840,15 +1851,15 @@
       <c r="Q21" s="4"/>
       <c r="R21" s="4"/>
       <c r="S21" s="4"/>
-      <c r="T21" s="4">
-        <v>1</v>
-      </c>
-      <c r="U21" s="4"/>
+      <c r="T21" s="4"/>
+      <c r="U21" s="4">
+        <v>1</v>
+      </c>
       <c r="V21" s="5"/>
-      <c r="W21" s="5"/>
-      <c r="X21" s="5">
-        <v>1</v>
-      </c>
+      <c r="W21" s="5">
+        <v>1</v>
+      </c>
+      <c r="X21" s="5"/>
       <c r="Y21" s="5"/>
       <c r="Z21" s="5"/>
       <c r="AA21" s="4"/>
@@ -1856,10 +1867,10 @@
         <v>1</v>
       </c>
       <c r="AC21" s="5"/>
-      <c r="AD21" s="5">
-        <v>1</v>
-      </c>
-      <c r="AE21" s="5"/>
+      <c r="AD21" s="5"/>
+      <c r="AE21" s="5">
+        <v>1</v>
+      </c>
       <c r="AF21" s="4"/>
       <c r="AG21" s="4">
         <v>1</v>
@@ -1874,7 +1885,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="9">
-        <v>19287</v>
+        <v>42114</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="4"/>
@@ -1886,10 +1897,10 @@
         <v>1</v>
       </c>
       <c r="J22" s="7"/>
-      <c r="K22" s="5">
-        <v>1</v>
-      </c>
-      <c r="L22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5">
+        <v>1</v>
+      </c>
       <c r="M22" s="5"/>
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
@@ -1897,15 +1908,15 @@
       <c r="Q22" s="4"/>
       <c r="R22" s="4"/>
       <c r="S22" s="4"/>
-      <c r="T22" s="4"/>
-      <c r="U22" s="4">
-        <v>1</v>
-      </c>
+      <c r="T22" s="4">
+        <v>1</v>
+      </c>
+      <c r="U22" s="4"/>
       <c r="V22" s="5"/>
-      <c r="W22" s="5">
-        <v>1</v>
-      </c>
-      <c r="X22" s="5"/>
+      <c r="W22" s="5"/>
+      <c r="X22" s="5">
+        <v>1</v>
+      </c>
       <c r="Y22" s="5"/>
       <c r="Z22" s="5"/>
       <c r="AA22" s="4"/>
@@ -1928,11 +1939,9 @@
     </row>
     <row r="23" spans="1:35">
       <c r="A23" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" s="9">
-        <v>42114</v>
-      </c>
+        <v>62</v>
+      </c>
+      <c r="B23" s="9"/>
       <c r="C23" s="7"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
@@ -1944,11 +1953,11 @@
       </c>
       <c r="J23" s="7"/>
       <c r="K23" s="5"/>
-      <c r="L23" s="5">
-        <v>1</v>
-      </c>
+      <c r="L23" s="5"/>
       <c r="M23" s="5"/>
-      <c r="N23" s="5"/>
+      <c r="N23" s="5">
+        <v>1</v>
+      </c>
       <c r="O23" s="5"/>
       <c r="P23" s="7"/>
       <c r="Q23" s="4"/>
@@ -1965,27 +1974,27 @@
       </c>
       <c r="Y23" s="5"/>
       <c r="Z23" s="5"/>
-      <c r="AA23" s="4"/>
-      <c r="AB23" s="4">
-        <v>1</v>
-      </c>
-      <c r="AC23" s="5"/>
+      <c r="AA23" s="4">
+        <v>1</v>
+      </c>
+      <c r="AB23" s="4"/>
+      <c r="AC23" s="5">
+        <v>1</v>
+      </c>
       <c r="AD23" s="5"/>
-      <c r="AE23" s="5">
-        <v>1</v>
-      </c>
+      <c r="AE23" s="5"/>
       <c r="AF23" s="4"/>
       <c r="AG23" s="4">
         <v>1</v>
       </c>
-      <c r="AH23" s="5"/>
-      <c r="AI23" s="5">
-        <v>1</v>
-      </c>
+      <c r="AH23" s="5">
+        <v>1</v>
+      </c>
+      <c r="AI23" s="5"/>
     </row>
     <row r="24" spans="1:35">
       <c r="A24" s="10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B24" s="9"/>
       <c r="C24" s="7"/>
@@ -2015,20 +2024,20 @@
       <c r="U24" s="4"/>
       <c r="V24" s="5"/>
       <c r="W24" s="5"/>
-      <c r="X24" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y24" s="5"/>
+      <c r="X24" s="5"/>
+      <c r="Y24" s="5">
+        <v>1</v>
+      </c>
       <c r="Z24" s="5"/>
       <c r="AA24" s="4">
         <v>1</v>
       </c>
       <c r="AB24" s="4"/>
-      <c r="AC24" s="5">
-        <v>1</v>
-      </c>
+      <c r="AC24" s="5"/>
       <c r="AD24" s="5"/>
-      <c r="AE24" s="5"/>
+      <c r="AE24" s="5">
+        <v>1</v>
+      </c>
       <c r="AF24" s="4"/>
       <c r="AG24" s="4">
         <v>1</v>
@@ -2040,18 +2049,18 @@
     </row>
     <row r="25" spans="1:35">
       <c r="A25" s="10" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B25" s="9"/>
       <c r="C25" s="7"/>
       <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
+      <c r="E25" s="4">
+        <v>1</v>
+      </c>
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
-      <c r="I25" s="4">
-        <v>1</v>
-      </c>
+      <c r="I25" s="4"/>
       <c r="J25" s="7"/>
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
@@ -2084,10 +2093,10 @@
       <c r="AE25" s="5">
         <v>1</v>
       </c>
-      <c r="AF25" s="4"/>
-      <c r="AG25" s="4">
-        <v>1</v>
-      </c>
+      <c r="AF25" s="4">
+        <v>1</v>
+      </c>
+      <c r="AG25" s="4"/>
       <c r="AH25" s="5">
         <v>1</v>
       </c>
@@ -2095,18 +2104,18 @@
     </row>
     <row r="26" spans="1:35">
       <c r="A26" s="10" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B26" s="9"/>
       <c r="C26" s="7"/>
       <c r="D26" s="4"/>
-      <c r="E26" s="4">
-        <v>1</v>
-      </c>
+      <c r="E26" s="4"/>
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
+      <c r="I26" s="4">
+        <v>1</v>
+      </c>
       <c r="J26" s="7"/>
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
@@ -2119,49 +2128,49 @@
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
       <c r="S26" s="4"/>
-      <c r="T26" s="4">
-        <v>1</v>
-      </c>
-      <c r="U26" s="4"/>
+      <c r="T26" s="4"/>
+      <c r="U26" s="4">
+        <v>1</v>
+      </c>
       <c r="V26" s="5"/>
-      <c r="W26" s="5"/>
+      <c r="W26" s="5">
+        <v>1</v>
+      </c>
       <c r="X26" s="5"/>
-      <c r="Y26" s="5">
-        <v>1</v>
-      </c>
+      <c r="Y26" s="5"/>
       <c r="Z26" s="5"/>
-      <c r="AA26" s="4">
-        <v>1</v>
-      </c>
-      <c r="AB26" s="4"/>
+      <c r="AA26" s="4"/>
+      <c r="AB26" s="4">
+        <v>1</v>
+      </c>
       <c r="AC26" s="5"/>
       <c r="AD26" s="5"/>
       <c r="AE26" s="5">
         <v>1</v>
       </c>
-      <c r="AF26" s="4">
-        <v>1</v>
-      </c>
-      <c r="AG26" s="4"/>
-      <c r="AH26" s="5">
-        <v>1</v>
-      </c>
-      <c r="AI26" s="5"/>
+      <c r="AF26" s="4"/>
+      <c r="AG26" s="4">
+        <v>1</v>
+      </c>
+      <c r="AH26" s="5"/>
+      <c r="AI26" s="5">
+        <v>1</v>
+      </c>
     </row>
     <row r="27" spans="1:35">
       <c r="A27" s="10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B27" s="9"/>
       <c r="C27" s="7"/>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
+      <c r="G27" s="4">
+        <v>1</v>
+      </c>
       <c r="H27" s="4"/>
-      <c r="I27" s="4">
-        <v>1</v>
-      </c>
+      <c r="I27" s="4"/>
       <c r="J27" s="7"/>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
@@ -2179,10 +2188,10 @@
         <v>1</v>
       </c>
       <c r="V27" s="5"/>
-      <c r="W27" s="5">
-        <v>1</v>
-      </c>
-      <c r="X27" s="5"/>
+      <c r="W27" s="5"/>
+      <c r="X27" s="5">
+        <v>1</v>
+      </c>
       <c r="Y27" s="5"/>
       <c r="Z27" s="5"/>
       <c r="AA27" s="4"/>
@@ -2205,34 +2214,34 @@
     </row>
     <row r="28" spans="1:35">
       <c r="A28" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B28" s="9"/>
       <c r="C28" s="7"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
-      <c r="G28" s="4">
-        <v>1</v>
-      </c>
+      <c r="G28" s="4"/>
       <c r="H28" s="4"/>
-      <c r="I28" s="4"/>
+      <c r="I28" s="4">
+        <v>1</v>
+      </c>
       <c r="J28" s="7"/>
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
       <c r="M28" s="5"/>
-      <c r="N28" s="5">
-        <v>1</v>
-      </c>
-      <c r="O28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5">
+        <v>1</v>
+      </c>
       <c r="P28" s="7"/>
       <c r="Q28" s="4"/>
       <c r="R28" s="4"/>
       <c r="S28" s="4"/>
-      <c r="T28" s="4"/>
-      <c r="U28" s="4">
-        <v>1</v>
-      </c>
+      <c r="T28" s="4">
+        <v>1</v>
+      </c>
+      <c r="U28" s="4"/>
       <c r="V28" s="5"/>
       <c r="W28" s="5"/>
       <c r="X28" s="5">
@@ -2259,185 +2268,130 @@
       </c>
     </row>
     <row r="29" spans="1:35">
-      <c r="A29" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4">
-        <v>1</v>
-      </c>
-      <c r="J29" s="7"/>
-      <c r="K29" s="5"/>
-      <c r="L29" s="5"/>
-      <c r="M29" s="5"/>
-      <c r="N29" s="5"/>
-      <c r="O29" s="5">
-        <v>1</v>
-      </c>
-      <c r="P29" s="7"/>
-      <c r="Q29" s="4"/>
-      <c r="R29" s="4"/>
-      <c r="S29" s="4"/>
-      <c r="T29" s="4">
-        <v>1</v>
-      </c>
-      <c r="U29" s="4"/>
-      <c r="V29" s="5"/>
-      <c r="W29" s="5"/>
-      <c r="X29" s="5">
-        <v>1</v>
-      </c>
-      <c r="Y29" s="5"/>
-      <c r="Z29" s="5"/>
-      <c r="AA29" s="4"/>
-      <c r="AB29" s="4">
-        <v>1</v>
-      </c>
-      <c r="AC29" s="5"/>
-      <c r="AD29" s="5"/>
-      <c r="AE29" s="5">
-        <v>1</v>
-      </c>
-      <c r="AF29" s="4"/>
-      <c r="AG29" s="4">
-        <v>1</v>
-      </c>
-      <c r="AH29" s="5"/>
-      <c r="AI29" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:35">
-      <c r="C30" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D30" s="11">
-        <f>SUM(D2:D29)*100/28</f>
+      <c r="C29" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D29" s="11">
+        <f>SUM(D2:D28)*100/27</f>
         <v>0</v>
       </c>
-      <c r="E30" s="11">
-        <f t="shared" ref="E30:I30" si="0">SUM(E2:E29)*100/28</f>
-        <v>3.5714285714285716</v>
-      </c>
-      <c r="F30" s="11">
-        <f t="shared" si="0"/>
+      <c r="E29" s="11">
+        <f>SUM(E2:E28)*100/27</f>
+        <v>3.7037037037037037</v>
+      </c>
+      <c r="F29" s="11">
+        <f>SUM(F2:F28)*100/27</f>
         <v>0</v>
       </c>
-      <c r="G30" s="11">
-        <f t="shared" si="0"/>
-        <v>3.5714285714285716</v>
-      </c>
-      <c r="H30" s="11">
-        <f t="shared" si="0"/>
+      <c r="G29" s="11">
+        <f>SUM(G2:G28)*100/27</f>
+        <v>3.7037037037037037</v>
+      </c>
+      <c r="H29" s="11">
+        <f>SUM(H2:H28)*100/28</f>
         <v>0</v>
       </c>
-      <c r="I30" s="11">
-        <f t="shared" si="0"/>
-        <v>92.857142857142861</v>
-      </c>
-      <c r="J30" s="11"/>
-      <c r="K30" s="11">
-        <f t="shared" ref="K30:O30" si="1">SUM(K2:K29)*100/28</f>
-        <v>60.714285714285715</v>
-      </c>
-      <c r="L30" s="11">
-        <f t="shared" si="1"/>
-        <v>14.285714285714286</v>
-      </c>
-      <c r="M30" s="11">
-        <f t="shared" si="1"/>
+      <c r="I29" s="11">
+        <f>SUM(I2:I28)*100/27</f>
+        <v>92.592592592592595</v>
+      </c>
+      <c r="J29" s="11"/>
+      <c r="K29" s="11">
+        <f>SUM(K2:K28)*100/27</f>
+        <v>62.962962962962962</v>
+      </c>
+      <c r="L29" s="11">
+        <f>SUM(L2:L28)*100/27</f>
+        <v>14.814814814814815</v>
+      </c>
+      <c r="M29" s="11">
+        <f>SUM(M2:M28)*100/28</f>
         <v>0</v>
       </c>
-      <c r="N30" s="11">
-        <f t="shared" si="1"/>
-        <v>17.857142857142858</v>
-      </c>
-      <c r="O30" s="11">
-        <f t="shared" si="1"/>
-        <v>3.5714285714285716</v>
-      </c>
-      <c r="P30" s="11"/>
-      <c r="Q30" s="11">
-        <f t="shared" ref="Q30:AI30" si="2">SUM(Q2:Q29)*100/28</f>
+      <c r="N29" s="11">
+        <f>SUM(N2:N28)*100/27</f>
+        <v>18.518518518518519</v>
+      </c>
+      <c r="O29" s="11">
+        <f>SUM(O2:O28)*100/27</f>
+        <v>3.7037037037037037</v>
+      </c>
+      <c r="P29" s="11"/>
+      <c r="Q29" s="11">
+        <f>SUM(Q2:Q28)*100/28</f>
         <v>0</v>
       </c>
-      <c r="R30" s="11">
-        <f t="shared" si="2"/>
+      <c r="R29" s="11">
+        <f>SUM(R2:R28)*100/28</f>
         <v>0</v>
       </c>
-      <c r="S30" s="11">
-        <f t="shared" si="2"/>
-        <v>3.5714285714285716</v>
-      </c>
-      <c r="T30" s="11">
-        <f t="shared" si="2"/>
-        <v>60.714285714285715</v>
-      </c>
-      <c r="U30" s="11">
-        <f t="shared" si="2"/>
-        <v>32.142857142857146</v>
-      </c>
-      <c r="V30" s="11">
-        <f t="shared" si="2"/>
+      <c r="S29" s="11">
+        <f>SUM(S2:S28)*100/27</f>
+        <v>3.7037037037037037</v>
+      </c>
+      <c r="T29" s="11">
+        <f>SUM(T2:T28)*100/27</f>
+        <v>62.962962962962962</v>
+      </c>
+      <c r="U29" s="11">
+        <f>SUM(U2:U28)*100/27</f>
+        <v>33.333333333333336</v>
+      </c>
+      <c r="V29" s="11">
+        <f>SUM(V2:V28)*100/28</f>
         <v>0</v>
       </c>
-      <c r="W30" s="11">
-        <f t="shared" si="2"/>
-        <v>25</v>
-      </c>
-      <c r="X30" s="11">
-        <f t="shared" si="2"/>
-        <v>60.714285714285715</v>
-      </c>
-      <c r="Y30" s="11">
-        <f t="shared" si="2"/>
-        <v>10.714285714285714</v>
-      </c>
-      <c r="Z30" s="11">
-        <f t="shared" si="2"/>
+      <c r="W29" s="11">
+        <f>SUM(W2:W28)*100/27</f>
+        <v>25.925925925925927</v>
+      </c>
+      <c r="X29" s="11">
+        <f>SUM(X2:X28)*100/27</f>
+        <v>62.962962962962962</v>
+      </c>
+      <c r="Y29" s="11">
+        <f>SUM(Y2:Y28)*100/27</f>
+        <v>11.111111111111111</v>
+      </c>
+      <c r="Z29" s="11">
+        <f>SUM(Z2:Z28)*100/28</f>
         <v>0</v>
       </c>
-      <c r="AA30" s="11">
-        <f t="shared" si="2"/>
-        <v>17.857142857142858</v>
-      </c>
-      <c r="AB30" s="11">
-        <f t="shared" si="2"/>
-        <v>78.571428571428569</v>
-      </c>
-      <c r="AC30" s="11">
-        <f t="shared" si="2"/>
-        <v>10.714285714285714</v>
-      </c>
-      <c r="AD30" s="11">
-        <f t="shared" si="2"/>
-        <v>21.428571428571427</v>
-      </c>
-      <c r="AE30" s="11">
-        <f t="shared" si="2"/>
-        <v>64.285714285714292</v>
-      </c>
-      <c r="AF30" s="11">
-        <f t="shared" si="2"/>
-        <v>10.714285714285714</v>
-      </c>
-      <c r="AG30" s="11">
-        <f t="shared" si="2"/>
-        <v>85.714285714285708</v>
-      </c>
-      <c r="AH30" s="11">
-        <f t="shared" si="2"/>
-        <v>14.285714285714286</v>
-      </c>
-      <c r="AI30" s="11">
-        <f t="shared" si="2"/>
-        <v>82.142857142857139</v>
+      <c r="AA29" s="11">
+        <f>SUM(AA2:AA28)*100/27</f>
+        <v>18.518518518518519</v>
+      </c>
+      <c r="AB29" s="11">
+        <f>SUM(AB2:AB28)*100/27</f>
+        <v>81.481481481481481</v>
+      </c>
+      <c r="AC29" s="11">
+        <f>SUM(AC2:AC28)*100/27</f>
+        <v>11.111111111111111</v>
+      </c>
+      <c r="AD29" s="11">
+        <f>SUM(AD2:AD28)*100/27</f>
+        <v>22.222222222222221</v>
+      </c>
+      <c r="AE29" s="11">
+        <f>SUM(AE2:AE28)*100/27</f>
+        <v>66.666666666666671</v>
+      </c>
+      <c r="AF29" s="11">
+        <f>SUM(AF2:AF28)*100/27</f>
+        <v>11.111111111111111</v>
+      </c>
+      <c r="AG29" s="11">
+        <f>SUM(AG2:AG28)*100/27</f>
+        <v>88.888888888888886</v>
+      </c>
+      <c r="AH29" s="11">
+        <f>SUM(AH2:AH28)*100/27</f>
+        <v>14.814814814814815</v>
+      </c>
+      <c r="AI29" s="11">
+        <f>SUM(AI2:AI28)*100/27</f>
+        <v>85.18518518518519</v>
       </c>
     </row>
   </sheetData>

</xml_diff>